<commit_message>
Homework01 with grid and population interpolation
</commit_message>
<xml_diff>
--- a/Assignments/SOC5670_Proj_DataDictionary.xlsx
+++ b/Assignments/SOC5670_Proj_DataDictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SOC5670\Assignments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SOC5670\Assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -141,6 +141,42 @@
   </si>
   <si>
     <t>Shapefile for the Springfield, Missouri MSA directional distribution of the White population.</t>
+  </si>
+  <si>
+    <t>sprfd_mo_msa_bndry</t>
+  </si>
+  <si>
+    <t>sprfd_mo_msa_grid00</t>
+  </si>
+  <si>
+    <t>Shapefile for the Springfield, Missouri MSA boundary.</t>
+  </si>
+  <si>
+    <t>sprfd_mo_msa_grid01</t>
+  </si>
+  <si>
+    <t>Shapefile for the Springfield, Missouri MSA with 1000x1000 meter grid.</t>
+  </si>
+  <si>
+    <t>sprfd_mo_msa_grid02</t>
+  </si>
+  <si>
+    <t>sprfd_mo_msa_int00</t>
+  </si>
+  <si>
+    <t>sprfd_mo_msa_int01</t>
+  </si>
+  <si>
+    <t>Shapefile for the Springfield, Missouri MSA with grid intersected with counties.</t>
+  </si>
+  <si>
+    <t>Shapefile for the Springield, Missouri MSA with population interpolated to grid in field sum_pop_grid.</t>
+  </si>
+  <si>
+    <t>Shapefile for the Springfield, Missouri MSA with grid intersected with counties and sum_grid_area field added.</t>
+  </si>
+  <si>
+    <t>Shapefile for the Springfield, Missouri MSA with grid clipped to boundary (grids less than 50,000 sq mtrs removed).</t>
   </si>
 </sst>
 </file>
@@ -521,18 +557,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" style="5" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="100.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="125.7109375" style="6" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
@@ -745,6 +781,72 @@
         <v>36</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>43887</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>43887</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>43887</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>43887</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>43887</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>43887</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Re-calculated grid populations for Springfield, Missouri MSA
</commit_message>
<xml_diff>
--- a/Assignments/SOC5670_Proj_DataDictionary.xlsx
+++ b/Assignments/SOC5670_Proj_DataDictionary.xlsx
@@ -170,13 +170,13 @@
     <t>Shapefile for the Springfield, Missouri MSA with grid intersected with counties.</t>
   </si>
   <si>
-    <t>Shapefile for the Springield, Missouri MSA with population interpolated to grid in field sum_pop_grid.</t>
-  </si>
-  <si>
     <t>Shapefile for the Springfield, Missouri MSA with grid intersected with counties and sum_grid_area field added.</t>
   </si>
   <si>
     <t>Shapefile for the Springfield, Missouri MSA with grid clipped to boundary (grids less than 50,000 sq mtrs removed).</t>
+  </si>
+  <si>
+    <t>Shapefile for the Springield, Missouri MSA with populations interpolated to grid in field sum_pop_grid, sum_blk_grid, sum_lat_grid, sum_wht_grid (overwritten with corrected calculation on 10-Mar-2020; reference Homework01_workflow03.mxd).</t>
   </si>
 </sst>
 </file>
@@ -560,7 +560,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -811,7 +811,7 @@
         <v>42</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -833,10 +833,10 @@
         <v>46</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>43887</v>
       </c>
@@ -844,7 +844,7 @@
         <v>44</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated data dictionary and formatted spreadsheet for tables
</commit_message>
<xml_diff>
--- a/Assignments/SOC5670_Proj_DataDictionary.xlsx
+++ b/Assignments/SOC5670_Proj_DataDictionary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
   <si>
     <t>Date</t>
   </si>
@@ -177,6 +177,63 @@
   </si>
   <si>
     <t>Shapefile for the Springield, Missouri MSA with populations interpolated to grid in field sum_pop_grid, sum_blk_grid, sum_lat_grid, sum_wht_grid (overwritten with corrected calculation on 10-Mar-2020; reference Homework01_workflow03.mxd).</t>
+  </si>
+  <si>
+    <t>sprfd_mo_msa_ct_04_spatAuto_global_blk.png</t>
+  </si>
+  <si>
+    <t>sprfd_mo_msa_ct_04_spatAuto_global_edtot.png</t>
+  </si>
+  <si>
+    <t>sprfd_mo_msa_ct_04_spatAuto_global_mhi.png</t>
+  </si>
+  <si>
+    <t>sprfd_mo_msa_ct_04_spatAuto_global_nhi.png</t>
+  </si>
+  <si>
+    <t>sprfd_mo_msa_ct_04_spatAuto_global_pblk.png</t>
+  </si>
+  <si>
+    <t>sprfd_mo_msa_ct_04_spatAuto_global_pov.png</t>
+  </si>
+  <si>
+    <t>sprfd_mo_msa_ct_04_spatAuto_global_pwht.png</t>
+  </si>
+  <si>
+    <t>sprfd_mo_msa_ct_04_spatAuto_global_wht.png</t>
+  </si>
+  <si>
+    <t>sprfd_mo_msa_grid02_spatAuto_global_blk.png</t>
+  </si>
+  <si>
+    <t>sprfd_mo_msa_grid02_spatAuto_global_wht.png</t>
+  </si>
+  <si>
+    <t>Univariate global Moran's I for white population at census tract level.</t>
+  </si>
+  <si>
+    <t>Univariate global Moran's I for no health insurance at census tract level.</t>
+  </si>
+  <si>
+    <t>Univariate global Moran's I for median household income at census tract level.</t>
+  </si>
+  <si>
+    <t>Univariate global Moran's I for total education at census tract level.</t>
+  </si>
+  <si>
+    <t>Univariate global Moran's I for percent black population at census tract level.</t>
+  </si>
+  <si>
+    <t>Univariate global Moran's I for poverty level at census tract level.</t>
+  </si>
+  <si>
+    <t>Univariate global Moran's I for percent white population at census tract level.</t>
+  </si>
+  <si>
+    <t>Univariate global Moran's I for black population at grid level.</t>
+  </si>
+  <si>
+    <t>Univariate global Moran's I for white population at grid level.</t>
   </si>
 </sst>
 </file>
@@ -557,17 +614,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" style="6" customWidth="1"/>
     <col min="3" max="3" width="125.7109375" style="6" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="4"/>
   </cols>
@@ -594,7 +651,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>43877</v>
       </c>
@@ -845,6 +902,116 @@
       </c>
       <c r="C25" s="6" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>43900</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>43900</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>43900</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>43900</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>43900</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>43900</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>43900</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>43900</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>43900</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>43900</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>